<commit_message>
juntar bruto con cluster para k:2,3,4
</commit_message>
<xml_diff>
--- a/analisis_consumos/logs/24_meses/sin_LFZA_FJAG/clusters_automaticos/Resumen_24_meses_sin2_clustes_automaticos.xlsx
+++ b/analisis_consumos/logs/24_meses/sin_LFZA_FJAG/clusters_automaticos/Resumen_24_meses_sin2_clustes_automaticos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos Boj\Desktop\GitHub-TFM\analisis_consumos\logs\24_meses\sin_LFZA_FJAG\clusters_automaticos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EC0E3B-F469-439C-8609-89CD023B80D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50708084-6C8A-49CA-B437-6675956193AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F60BFC8B-6EFF-448C-80BF-F645298F57E9}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{F60BFC8B-6EFF-448C-80BF-F645298F57E9}"/>
   </bookViews>
   <sheets>
     <sheet name="resumen" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="215">
   <si>
     <t>JACL</t>
   </si>
@@ -1211,14 +1211,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1662,9 +1661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6732A438-33AA-41FF-ACDC-B7B119E1E5AD}">
   <dimension ref="A1:BC41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH28" sqref="AH28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,10 +1801,10 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>44927</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>44958</v>
       </c>
       <c r="D6" s="5">
@@ -1817,13 +1816,13 @@
       <c r="F6" s="5">
         <v>45047</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>45078</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>45108</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>45139</v>
       </c>
       <c r="J6" s="5">
@@ -1835,13 +1834,13 @@
       <c r="L6" s="5">
         <v>45231</v>
       </c>
-      <c r="M6" s="10">
+      <c r="M6" s="9">
         <v>45261</v>
       </c>
-      <c r="N6" s="10">
+      <c r="N6" s="9">
         <v>45292</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>45323</v>
       </c>
       <c r="P6" s="5">
@@ -1853,13 +1852,13 @@
       <c r="R6" s="5">
         <v>45413</v>
       </c>
-      <c r="S6" s="9">
+      <c r="S6" s="8">
         <v>45444</v>
       </c>
-      <c r="T6" s="9">
+      <c r="T6" s="8">
         <v>45474</v>
       </c>
-      <c r="U6" s="9">
+      <c r="U6" s="8">
         <v>45505</v>
       </c>
       <c r="V6" s="5">
@@ -1871,7 +1870,7 @@
       <c r="X6" s="5">
         <v>45597</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Y6" s="9">
         <v>45627</v>
       </c>
       <c r="Z6" s="5"/>
@@ -1956,7 +1955,7 @@
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="1">
         <v>1</v>
       </c>
@@ -2026,16 +2025,19 @@
       <c r="Y7" s="4">
         <v>0</v>
       </c>
-      <c r="AA7" s="6">
+      <c r="Z7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA7">
         <v>8</v>
       </c>
-      <c r="AB7" s="6">
+      <c r="AB7">
         <v>6</v>
       </c>
-      <c r="AC7" s="6">
+      <c r="AC7">
         <v>3</v>
       </c>
-      <c r="AD7" s="6">
+      <c r="AD7">
         <v>6</v>
       </c>
       <c r="AE7" t="s">
@@ -2191,16 +2193,19 @@
       <c r="Y8" s="2">
         <v>1</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="Z8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA8">
         <v>10</v>
       </c>
-      <c r="AB8" s="6">
-        <v>2</v>
-      </c>
-      <c r="AC8" s="6">
-        <v>2</v>
-      </c>
-      <c r="AD8" s="6">
+      <c r="AB8">
+        <v>2</v>
+      </c>
+      <c r="AC8">
+        <v>2</v>
+      </c>
+      <c r="AD8">
         <v>10</v>
       </c>
       <c r="AE8" t="s">
@@ -2284,20 +2289,20 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
       <c r="P9" s="1">
         <v>3</v>
       </c>
@@ -2328,14 +2333,16 @@
       <c r="Y9" s="4">
         <v>0</v>
       </c>
+      <c r="Z9" t="s">
+        <v>5</v>
+      </c>
       <c r="AA9" s="3">
         <v>7</v>
       </c>
-      <c r="AB9" s="6">
-        <v>2</v>
-      </c>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="6">
+      <c r="AB9">
+        <v>2</v>
+      </c>
+      <c r="AD9">
         <v>1</v>
       </c>
       <c r="AE9" t="s">
@@ -2415,120 +2422,122 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
-      <c r="AA10" s="8"/>
-      <c r="AB10" s="8"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
-      <c r="AE10" s="8"/>
-      <c r="AF10" s="8" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="AG10" s="8">
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG10" s="7">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AH10" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="8">
-        <v>1</v>
-      </c>
-      <c r="AL10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="8">
-        <v>1</v>
-      </c>
-      <c r="AN10" s="8" t="s">
+      <c r="AH10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="7">
+        <v>1</v>
+      </c>
+      <c r="AN10" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AO10" s="8" t="s">
+      <c r="AO10" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AP10" s="8" t="s">
+      <c r="AP10" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AQ10" s="8">
+      <c r="AQ10" s="7">
         <v>56</v>
       </c>
-      <c r="AR10" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AS10" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AT10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AV10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AW10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AX10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AY10" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AZ10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="BA10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="BB10" s="8" t="s">
+      <c r="AR10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AS10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AV10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AW10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AX10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AY10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AZ10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="BA10" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB10" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="BC10" s="8" t="s">
+      <c r="BC10" s="7" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
       <c r="D11" s="3">
         <v>2</v>
       </c>
@@ -2595,19 +2604,22 @@
       <c r="Y11" s="4">
         <v>0</v>
       </c>
+      <c r="Z11" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="AA11" s="3">
         <v>10</v>
       </c>
-      <c r="AB11" s="6">
+      <c r="AB11">
         <v>5</v>
       </c>
-      <c r="AC11" s="6">
+      <c r="AC11">
         <v>4</v>
       </c>
-      <c r="AD11" s="6">
+      <c r="AD11">
         <v>3</v>
       </c>
-      <c r="AE11" s="6" t="s">
+      <c r="AE11" t="s">
         <v>206</v>
       </c>
       <c r="AF11" s="3" t="s">
@@ -2684,7 +2696,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2760,16 +2772,19 @@
       <c r="Y12" s="4">
         <v>0</v>
       </c>
+      <c r="Z12" t="s">
+        <v>8</v>
+      </c>
       <c r="AA12" s="3">
         <v>15</v>
       </c>
-      <c r="AB12" s="6">
+      <c r="AB12">
         <v>6</v>
       </c>
-      <c r="AD12" s="6">
+      <c r="AD12">
         <v>3</v>
       </c>
-      <c r="AE12" s="6" t="s">
+      <c r="AE12" t="s">
         <v>208</v>
       </c>
       <c r="AF12" t="s">
@@ -2846,7 +2861,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -2922,16 +2937,19 @@
       <c r="Y13" s="4">
         <v>0</v>
       </c>
+      <c r="Z13" t="s">
+        <v>0</v>
+      </c>
       <c r="AA13" s="3">
         <v>22</v>
       </c>
-      <c r="AC13" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD13" s="6">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="6" t="s">
+      <c r="AC13">
+        <v>1</v>
+      </c>
+      <c r="AD13">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="s">
         <v>212</v>
       </c>
       <c r="AF13" t="s">
@@ -3008,7 +3026,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3084,16 +3102,19 @@
       <c r="Y14" s="4">
         <v>0</v>
       </c>
-      <c r="AA14" s="6">
+      <c r="Z14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14">
         <v>4</v>
       </c>
-      <c r="AC14" s="6">
+      <c r="AC14">
         <v>7</v>
       </c>
       <c r="AD14" s="3">
         <v>13</v>
       </c>
-      <c r="AE14" s="6" t="s">
+      <c r="AE14" t="s">
         <v>207</v>
       </c>
       <c r="AF14" t="s">
@@ -3170,7 +3191,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -3246,13 +3267,16 @@
       <c r="Y15" s="4">
         <v>0</v>
       </c>
+      <c r="Z15" t="s">
+        <v>9</v>
+      </c>
       <c r="AA15" s="3">
         <v>23</v>
       </c>
-      <c r="AC15" s="6">
-        <v>1</v>
-      </c>
-      <c r="AE15" s="6" t="s">
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
         <v>212</v>
       </c>
       <c r="AF15" t="s">
@@ -3329,7 +3353,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -3405,19 +3429,22 @@
       <c r="Y16" s="4">
         <v>0</v>
       </c>
-      <c r="AA16" s="6">
+      <c r="Z16" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA16">
         <v>3</v>
       </c>
-      <c r="AB16" s="6">
+      <c r="AB16">
         <v>4</v>
       </c>
-      <c r="AC16" s="6">
+      <c r="AC16">
         <v>2</v>
       </c>
       <c r="AD16" s="3">
         <v>15</v>
       </c>
-      <c r="AE16" s="6" t="s">
+      <c r="AE16" t="s">
         <v>212</v>
       </c>
       <c r="AF16" t="s">
@@ -3494,111 +3521,113 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:55" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="8"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="AG17" s="8">
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG17" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AH17" s="8">
-        <v>1</v>
-      </c>
-      <c r="AI17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN17" s="8" t="s">
+      <c r="AH17" s="7">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="AO17" s="8" t="s">
+      <c r="AO17" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AP17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AQ17" s="8">
+      <c r="AP17" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AQ17" s="7">
         <v>68</v>
       </c>
-      <c r="AR17" s="8" t="s">
+      <c r="AR17" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AS17" s="8" t="s">
+      <c r="AS17" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="AT17" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AU17" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AV17" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AW17" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AX17" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="AY17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="AZ17" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="BA17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="BB17" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="BC17" s="8" t="s">
+      <c r="AT17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AV17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AW17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AX17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="AY17" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AZ17" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="BA17" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BB17" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC17" s="7" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3678,19 +3707,22 @@
       <c r="Y18" s="4">
         <v>0</v>
       </c>
-      <c r="AA18" s="6">
-        <v>2</v>
-      </c>
-      <c r="AB18" s="6">
+      <c r="Z18" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA18">
+        <v>2</v>
+      </c>
+      <c r="AB18">
         <v>4</v>
       </c>
-      <c r="AC18" s="6">
+      <c r="AC18">
         <v>5</v>
       </c>
       <c r="AD18" s="3">
         <v>13</v>
       </c>
-      <c r="AE18" s="6" t="s">
+      <c r="AE18" t="s">
         <v>214</v>
       </c>
       <c r="AF18" t="s">
@@ -3843,16 +3875,19 @@
       <c r="Y19" s="4">
         <v>0</v>
       </c>
+      <c r="Z19" t="s">
+        <v>13</v>
+      </c>
       <c r="AA19" s="3">
         <v>10</v>
       </c>
-      <c r="AB19" s="6">
+      <c r="AB19">
         <v>6</v>
       </c>
-      <c r="AC19" s="6">
+      <c r="AC19">
         <v>3</v>
       </c>
-      <c r="AD19" s="6">
+      <c r="AD19">
         <v>5</v>
       </c>
       <c r="AE19" t="s">
@@ -3933,39 +3968,39 @@
       </c>
     </row>
     <row r="20" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
       <c r="Y20" s="2">
         <v>1</v>
       </c>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6">
+      <c r="Z20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD20">
         <v>1</v>
       </c>
       <c r="AE20" t="s">
@@ -4049,7 +4084,7 @@
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21" s="7"/>
       <c r="C21" s="1">
         <v>1</v>
       </c>
@@ -4119,13 +4154,16 @@
       <c r="Y21" s="4">
         <v>0</v>
       </c>
-      <c r="AA21" s="6">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="6">
+      <c r="Z21" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA21">
+        <v>1</v>
+      </c>
+      <c r="AB21">
         <v>4</v>
       </c>
-      <c r="AC21" s="6">
+      <c r="AC21">
         <v>5</v>
       </c>
       <c r="AD21" s="3">
@@ -4215,7 +4253,7 @@
       <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>0</v>
       </c>
       <c r="D22" s="2">
@@ -4284,13 +4322,16 @@
       <c r="Y22" s="2">
         <v>1</v>
       </c>
-      <c r="AA22" s="6">
+      <c r="Z22" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA22">
         <v>3</v>
       </c>
-      <c r="AB22" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC22" s="6">
+      <c r="AB22">
+        <v>1</v>
+      </c>
+      <c r="AC22">
         <v>7</v>
       </c>
       <c r="AD22" s="3">
@@ -4449,12 +4490,12 @@
       <c r="Y23" s="4">
         <v>0</v>
       </c>
+      <c r="Z23" t="s">
+        <v>15</v>
+      </c>
       <c r="AA23" s="3">
         <v>18</v>
       </c>
-      <c r="AB23" s="6"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
       <c r="AE23" t="s">
         <v>212</v>
       </c>
@@ -4608,11 +4649,13 @@
       <c r="Y24" s="4">
         <v>0</v>
       </c>
-      <c r="AA24" s="6">
+      <c r="Z24" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA24">
         <v>5</v>
       </c>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="6">
+      <c r="AC24">
         <v>3</v>
       </c>
       <c r="AD24" s="3">
@@ -4695,12 +4738,6 @@
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="6"/>
-    </row>
     <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="B26">
         <f>COUNTA(B27:B30)</f>
@@ -4738,7 +4775,7 @@
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -4957,7 +4994,6 @@
       <c r="A29" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="6"/>
       <c r="C29" s="2" t="s">
         <v>31</v>
       </c>
@@ -4991,35 +5027,17 @@
       <c r="Q29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
-      <c r="V29" s="6"/>
-      <c r="W29" s="6"/>
-      <c r="X29" s="6"/>
-      <c r="Y29" s="6"/>
     </row>
     <row r="30" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="6"/>
       <c r="C30" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
       <c r="L30" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M30" s="6"/>
       <c r="N30" s="4" t="s">
         <v>48</v>
       </c>
@@ -5032,53 +5050,45 @@
       <c r="Q30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
     </row>
     <row r="31" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" t="s">
         <v>66</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" t="s">
         <v>83</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="G31" t="s">
         <v>85</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H31" t="s">
         <v>90</v>
       </c>
       <c r="I31" t="s">
         <v>132</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="J31" t="s">
         <v>94</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="K31" t="s">
         <v>94</v>
       </c>
-      <c r="L31" s="6" t="s">
+      <c r="L31" t="s">
         <v>35</v>
       </c>
-      <c r="M31" s="6" t="s">
+      <c r="M31" t="s">
         <v>103</v>
       </c>
       <c r="N31" t="s">
@@ -5093,26 +5103,25 @@
       <c r="Q31" t="s">
         <v>54</v>
       </c>
-      <c r="R31" s="6" t="s">
+      <c r="R31" t="s">
         <v>109</v>
       </c>
-      <c r="S31" s="6" t="s">
+      <c r="S31" t="s">
         <v>113</v>
       </c>
-      <c r="T31" s="6" t="s">
+      <c r="T31" t="s">
         <v>115</v>
       </c>
-      <c r="U31" s="6" t="s">
+      <c r="U31" t="s">
         <v>115</v>
       </c>
-      <c r="V31" s="6" t="s">
+      <c r="V31" t="s">
         <v>123</v>
       </c>
-      <c r="W31" s="6"/>
-      <c r="X31" s="6" t="s">
+      <c r="X31" t="s">
         <v>118</v>
       </c>
-      <c r="Y31" s="6" t="s">
+      <c r="Y31" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5120,40 +5129,40 @@
       <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" t="s">
         <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" t="s">
         <v>88</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" t="s">
         <v>92</v>
       </c>
       <c r="I32" t="s">
         <v>134</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" t="s">
         <v>96</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" t="s">
         <v>101</v>
       </c>
-      <c r="L32" s="6" t="s">
+      <c r="L32" t="s">
         <v>38</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="M32" t="s">
         <v>105</v>
       </c>
       <c r="N32" t="s">
@@ -5168,57 +5177,51 @@
       <c r="Q32" t="s">
         <v>34</v>
       </c>
-      <c r="R32" s="6" t="s">
+      <c r="R32" t="s">
         <v>111</v>
       </c>
-      <c r="S32" s="6" t="s">
+      <c r="S32" t="s">
         <v>115</v>
       </c>
-      <c r="T32" s="6" t="s">
+      <c r="T32" t="s">
         <v>118</v>
       </c>
-      <c r="U32" s="6" t="s">
+      <c r="U32" t="s">
         <v>121</v>
       </c>
-      <c r="V32" s="6" t="s">
+      <c r="V32" t="s">
         <v>115</v>
       </c>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6" t="s">
+      <c r="X32" t="s">
         <v>123</v>
       </c>
-      <c r="Y32" s="6" t="s">
+      <c r="Y32" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="6"/>
       <c r="C33" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" t="s">
         <v>81</v>
       </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
       <c r="I33" t="s">
         <v>136</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="J33" t="s">
         <v>98</v>
       </c>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6" t="s">
+      <c r="L33" t="s">
         <v>36</v>
       </c>
-      <c r="M33" s="6" t="s">
+      <c r="M33" t="s">
         <v>107</v>
       </c>
       <c r="N33" t="s">
@@ -5233,35 +5236,17 @@
       <c r="Q33" t="s">
         <v>62</v>
       </c>
-      <c r="R33" s="6"/>
-      <c r="S33" s="6"/>
-      <c r="T33" s="6"/>
-      <c r="U33" s="6"/>
-      <c r="V33" s="6"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="6"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="6"/>
       <c r="C34" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6" t="s">
+      <c r="L34" t="s">
         <v>34</v>
       </c>
-      <c r="M34" s="6"/>
       <c r="N34" t="s">
         <v>38</v>
       </c>
@@ -5274,46 +5259,26 @@
       <c r="Q34" t="s">
         <v>64</v>
       </c>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="6"/>
-      <c r="V34" s="6"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="6"/>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
       <c r="B38" s="4"/>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="1"/>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
       <c r="B40" s="3"/>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>21</v>
       </c>
@@ -5333,7 +5298,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5342,22 +5307,22 @@
       <c r="A1" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="8">
         <v>45078</v>
       </c>
-      <c r="C1" s="9">
+      <c r="C1" s="8">
         <v>45108</v>
       </c>
-      <c r="D1" s="9">
+      <c r="D1" s="8">
         <v>45139</v>
       </c>
-      <c r="E1" s="9">
+      <c r="E1" s="8">
         <v>45444</v>
       </c>
-      <c r="F1" s="9">
+      <c r="F1" s="8">
         <v>45474</v>
       </c>
-      <c r="G1" s="9">
+      <c r="G1" s="8">
         <v>45505</v>
       </c>
       <c r="H1" t="s">
@@ -5420,9 +5385,9 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="2">
         <v>1</v>
       </c>
@@ -5437,21 +5402,21 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="4">
@@ -5607,16 +5572,16 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7" t="s">
         <v>140</v>
       </c>
     </row>
@@ -5673,15 +5638,15 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="3" t="s">
         <v>142</v>
       </c>
@@ -5794,22 +5759,22 @@
       <c r="A22" t="s">
         <v>204</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="9">
         <v>44927</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>44958</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>45261</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>45292</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>45323</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>45627</v>
       </c>
       <c r="H22" t="s">
@@ -5820,7 +5785,7 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="7"/>
       <c r="C23" s="1">
         <v>1</v>
       </c>
@@ -5870,11 +5835,11 @@
       <c r="A25" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="4">
         <v>0</v>
       </c>
@@ -5883,25 +5848,25 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="4">
         <v>1</v>
       </c>
@@ -6049,16 +6014,16 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7" t="s">
         <v>147</v>
       </c>
     </row>
@@ -6115,14 +6080,14 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="2">
         <v>1</v>
       </c>
@@ -6134,7 +6099,7 @@
       <c r="A37" t="s">
         <v>17</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="7"/>
       <c r="C37" s="1">
         <v>1</v>
       </c>
@@ -6161,7 +6126,7 @@
       <c r="B38" s="2">
         <v>1</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>0</v>
       </c>
       <c r="D38" s="3">
@@ -6242,7 +6207,7 @@
   <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O19"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6380,7 +6345,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
@@ -6433,48 +6398,48 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>1</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>0</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>0</v>
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="7">
         <v>1</v>
       </c>
       <c r="J5">
         <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="7">
         <v>0</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="7">
         <v>1</v>
       </c>
       <c r="N5">
@@ -6483,7 +6448,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
@@ -6690,7 +6655,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O9" s="10" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6801,48 +6766,48 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" s="7">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
         <v>1</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>0</v>
       </c>
       <c r="F12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>0</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="7">
         <v>0</v>
       </c>
       <c r="N12">

</xml_diff>